<commit_message>
Second Test case added
</commit_message>
<xml_diff>
--- a/src/test/resources/ATS_LoginDetails.xlsx
+++ b/src/test/resources/ATS_LoginDetails.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\eclipse-workspace123\ATS_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7431EEE2-0B74-473B-BE49-548CB809B95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3039D-ED00-439C-87DF-53E06570AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>UserName</t>
   </si>
@@ -39,17 +39,84 @@
     <t>Neha@5678</t>
   </si>
   <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
     <t>Https://www.google.com/meet</t>
+  </si>
+  <si>
+    <t>Client Name</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>About Client</t>
+  </si>
+  <si>
+    <t>The human brain is powerful but subject to limitations. For this reason, we have evolved to have a collection of cognitive biases. These are systematic errors in thinking that occur when we process and interpret information around us, and it affects the decisions and judgments that we make.</t>
+  </si>
+  <si>
+    <t>One of these biases is overconfidence. This is the tendency we have to be more confident in our own abilities than is objectively reasonable.</t>
+  </si>
+  <si>
+    <t>The human brain is powerful but subject to limitations. 
+For this reason, we have evolved to have a collection of cognitive biases</t>
+  </si>
+  <si>
+    <t>Billing Street</t>
+  </si>
+  <si>
+    <t>Billing city</t>
+  </si>
+  <si>
+    <t>Billing state</t>
+  </si>
+  <si>
+    <t>Billing code</t>
+  </si>
+  <si>
+    <t>New Street</t>
+  </si>
+  <si>
+    <t>New City</t>
+  </si>
+  <si>
+    <t>Free state</t>
+  </si>
+  <si>
+    <t>461001</t>
+  </si>
+  <si>
+    <t>C:\Users\vijay\eclipse-workspace123\ATS_Project\src\test\resources\upload1.docx</t>
+  </si>
+  <si>
+    <t>C:\Users\vijay\eclipse-workspace123\ATS_Project\src\test\resources\upload2.docx</t>
+  </si>
+  <si>
+    <t>Software Engineer in Test</t>
+  </si>
+  <si>
+    <t>New Test Company</t>
+  </si>
+  <si>
+    <t>https://www.testdevcompany.com</t>
+  </si>
+  <si>
+    <t>7712674411</t>
+  </si>
+  <si>
+    <t>6675512341</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +129,18 @@
       <color rgb="FF2A00FF"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,11 +163,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,19 +455,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.54296875" customWidth="1"/>
     <col min="2" max="2" width="20.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6328125" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -398,14 +486,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Test cases Added also enhanced utility class
</commit_message>
<xml_diff>
--- a/src/test/resources/ATS_LoginDetails.xlsx
+++ b/src/test/resources/ATS_LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\eclipse-workspace123\ATS_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3039D-ED00-439C-87DF-53E06570AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEA73D8-DB09-4008-B8B7-EE3DE805AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>UserName</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>6675512341</t>
+  </si>
+  <si>
+    <t>super@admin.com</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,6 +492,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>

</xml_diff>